<commit_message>
file attachment gatein pre-Jose (21-Nov-22)
</commit_message>
<xml_diff>
--- a/Requirements/Requirments_v2.0.xlsx
+++ b/Requirements/Requirments_v2.0.xlsx
@@ -1106,7 +1106,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1394,8 +1394,8 @@
       <c r="C19" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>52</v>
+      <c r="D19" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="E19" s="4"/>
     </row>
@@ -1409,8 +1409,8 @@
       <c r="C20" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>52</v>
+      <c r="D20" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="E20" s="4"/>
     </row>

</xml_diff>

<commit_message>
Gate-In Pre file attachment - Jose (29-Nov-222)
</commit_message>
<xml_diff>
--- a/Requirements/Requirments_v2.0.xlsx
+++ b/Requirements/Requirments_v2.0.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="55">
   <si>
     <t>Capture Commodity details - Add in Gate-In Form (Change Stock Type to Commodity Type) (Garments, Auto Parts, Leather Garments, Shoe Uppers, Finish Leather, Console, Electrical &amp; Electronics) - Jose (Venkat to send commodity details list)</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>In Pre-Check-In, Attachment for customer approval (in case of mismatch)</t>
+  </si>
+  <si>
+    <t>WIP</t>
   </si>
 </sst>
 </file>
@@ -332,7 +335,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -521,6 +524,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -739,7 +748,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -778,6 +787,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1103,10 +1115,10 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
+      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1394,8 +1406,8 @@
       <c r="C19" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>47</v>
+      <c r="D19" s="15" t="s">
+        <v>54</v>
       </c>
       <c r="E19" s="4"/>
     </row>
@@ -1409,8 +1421,8 @@
       <c r="C20" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>47</v>
+      <c r="D20" s="15" t="s">
+        <v>54</v>
       </c>
       <c r="E20" s="4"/>
     </row>

</xml_diff>

<commit_message>
latest Commit - Jose (16-Dec-2022)
</commit_message>
<xml_diff>
--- a/Requirements/Requirments_v2.0.xlsx
+++ b/Requirements/Requirments_v2.0.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="58">
   <si>
     <t>Capture Commodity details - Add in Gate-In Form (Change Stock Type to Commodity Type) (Garments, Auto Parts, Leather Garments, Shoe Uppers, Finish Leather, Console, Electrical &amp; Electronics) - Jose (Venkat to send commodity details list)</t>
   </si>
@@ -186,7 +186,16 @@
     <t>In Pre-Check-In, Attachment for customer approval (in case of mismatch)</t>
   </si>
   <si>
-    <t>WIP</t>
+    <t>Hold</t>
+  </si>
+  <si>
+    <t>Recommend to implement this feature after go-live.</t>
+  </si>
+  <si>
+    <t>Since it has one to many releationship, technically its not advisable to create WH job from Pre-gatein form</t>
+  </si>
+  <si>
+    <t>Will be implemented during Go-Live</t>
   </si>
 </sst>
 </file>
@@ -335,7 +344,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -524,12 +533,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -788,7 +791,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1115,10 +1118,10 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1127,7 +1130,7 @@
     <col min="2" max="2" width="125.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1172,7 +1175,9 @@
       <c r="C3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="11"/>
+      <c r="D3" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="E3" s="13" t="s">
         <v>50</v>
       </c>
@@ -1202,7 +1207,9 @@
       <c r="C5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="11"/>
+      <c r="D5" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="E5" s="13" t="s">
         <v>51</v>
       </c>
@@ -1222,7 +1229,7 @@
       </c>
       <c r="E6" s="13"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1232,8 +1239,12 @@
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="4"/>
+      <c r="D7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
@@ -1275,7 +1286,7 @@
       <c r="C10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="15" t="s">
         <v>52</v>
       </c>
       <c r="E10" s="4"/>
@@ -1290,7 +1301,7 @@
       <c r="C11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="15" t="s">
         <v>52</v>
       </c>
       <c r="E11" s="4"/>
@@ -1305,7 +1316,7 @@
       <c r="C12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="15" t="s">
         <v>52</v>
       </c>
       <c r="E12" s="4"/>
@@ -1325,7 +1336,7 @@
       </c>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1336,9 +1347,11 @@
         <v>4</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
@@ -1378,7 +1391,9 @@
       <c r="C17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="D17" s="15" t="s">
+        <v>52</v>
+      </c>
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1406,8 +1421,8 @@
       <c r="C19" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="15" t="s">
-        <v>54</v>
+      <c r="D19" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="E19" s="4"/>
     </row>
@@ -1421,8 +1436,8 @@
       <c r="C20" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="15" t="s">
-        <v>54</v>
+      <c r="D20" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="E20" s="4"/>
     </row>
@@ -1436,7 +1451,9 @@
       <c r="C21" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="3"/>
+      <c r="D21" s="15" t="s">
+        <v>52</v>
+      </c>
       <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -1449,7 +1466,7 @@
       <c r="C22" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="15" t="s">
         <v>52</v>
       </c>
       <c r="E22" s="4"/>
@@ -1464,7 +1481,9 @@
       <c r="C23" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="3"/>
+      <c r="D23" s="15" t="s">
+        <v>52</v>
+      </c>
       <c r="E23" s="4"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1477,7 +1496,9 @@
       <c r="C24" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="3"/>
+      <c r="D24" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="E24" s="4"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1490,8 +1511,12 @@
       <c r="C25" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="4"/>
+      <c r="D25" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="3">

</xml_diff>